<commit_message>
Adjust stochastic example to actually be different for Scenario A & B
Fix issue installing mpi4py on unix systems
</commit_message>
<xml_diff>
--- a/data/exampleStochastic/Power_Network.xlsx
+++ b/data/exampleStochastic/Power_Network.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\exampleStochastic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597FC3C0-98E1-4755-9DF7-E0FB7125DFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F92F19-7763-4597-85E5-D10D8DE0ABC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="1" r:id="rId1"/>
     <sheet name="ScenarioB" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -209,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="88">
   <si>
     <t>Power - Network</t>
   </si>
@@ -2657,9 +2670,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12" t="s">
         <v>82</v>
@@ -2763,9 +2774,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
         <v>75</v>
@@ -2816,9 +2825,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12" t="s">
         <v>85</v>
@@ -2869,9 +2876,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12" t="s">
         <v>86</v>

</xml_diff>